<commit_message>
[siva]Add: Updated file is added
</commit_message>
<xml_diff>
--- a/FlipKart/Resources/Flipkart_DDT.xlsx
+++ b/FlipKart/Resources/Flipkart_DDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivaranjani.b\source\repos\FlipKart\FlipKart\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752EE578-0A9C-456C-B292-A4923B35DFDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AB889D-E4FC-4C97-8C91-A29881963E71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{22E06B59-9502-420F-BD6A-E7786F8E2852}"/>
   </bookViews>
@@ -69,8 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B39FF17-9949-46B6-8318-8709A0ADC652}">
-  <dimension ref="A4:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,19 +400,19 @@
     <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>8667361462</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[siva]Adding : code to find the rating of the products
</commit_message>
<xml_diff>
--- a/FlipKart/Resources/Flipkart_DDT.xlsx
+++ b/FlipKart/Resources/Flipkart_DDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivaranjani.b\source\repos\FlipKart\FlipKart\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCF0206-75CF-4356-B210-D050166A8242}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD396E9-5276-45B4-8214-062CD97E1B92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{22E06B59-9502-420F-BD6A-E7786F8E2852}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>email</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>sivabalaan10</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>mobiles</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B39FF17-9949-46B6-8318-8709A0ADC652}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,20 +406,26 @@
     <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>8667361462</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[siva]Refactoring : Code with validations
</commit_message>
<xml_diff>
--- a/FlipKart/Resources/Flipkart_DDT.xlsx
+++ b/FlipKart/Resources/Flipkart_DDT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivaranjani.b\source\repos\FlipKart\FlipKart\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD396E9-5276-45B4-8214-062CD97E1B92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5456F14-0F08-401B-BD3C-50CDF45DE034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{22E06B59-9502-420F-BD6A-E7786F8E2852}"/>
   </bookViews>
@@ -46,10 +46,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,16 +80,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,19 +405,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B39FF17-9949-46B6-8318-8709A0ADC652}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>8667361462</v>
       </c>
@@ -427,6 +439,7 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>